<commit_message>
AutoCommit_9 января 2024 г. 11:53:17_SibNout2023
</commit_message>
<xml_diff>
--- a/_2023-2024_2ИСИП-322_Дискретная математика с элементами математической логики_I семестр.xlsx
+++ b/_2023-2024_2ИСИП-322_Дискретная математика с элементами математической логики_I семестр.xlsx
@@ -533,10 +533,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>